<commit_message>
add: informe de horas completo
</commit_message>
<xml_diff>
--- a/Entrega 1/Documentacion/Registro de Horas.xlsx
+++ b/Entrega 1/Documentacion/Registro de Horas.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fiore/Documents/Ingeniería de Software Ágil 2/Obligatorio/obligatorio-mazziotti-macedo-torres/Entrega 1/Documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90BEE55E-3C46-7B47-8F35-0F04626C624D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DD36FA-2B10-49CF-B0C4-4FE7D070DBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19660" xr2:uid="{521A97D7-3E70-3344-99B1-188E39FB8E70}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>Integrante</t>
   </si>
@@ -66,6 +55,27 @@
   </si>
   <si>
     <t>Documentación</t>
+  </si>
+  <si>
+    <t>03:00 hs</t>
+  </si>
+  <si>
+    <t>02:00 hs</t>
+  </si>
+  <si>
+    <t>01:00 hs</t>
+  </si>
+  <si>
+    <t>Config. De Ambiente</t>
+  </si>
+  <si>
+    <t>Testing Exploratorio</t>
+  </si>
+  <si>
+    <t>03:30 hs</t>
+  </si>
+  <si>
+    <t>Análisis de Código</t>
   </si>
 </sst>
 </file>
@@ -73,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -112,23 +122,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -444,127 +463,324 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AF7156-946E-AA46-97A9-C1B7EDD3D508}">
-  <dimension ref="B1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="16.59765625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="6" width="16.6640625" style="1"/>
-    <col min="7" max="7" width="16.6640625" style="2"/>
+    <col min="4" max="4" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.59765625" style="1"/>
+    <col min="7" max="7" width="16.59765625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="3">
+    <row r="3" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="8">
         <v>45181.895138888889</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="8">
         <v>45182.020138888889</v>
       </c>
-      <c r="G3" s="6">
-        <f>F3-E3</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
+      <c r="G3" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9"/>
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9"/>
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5">
+      <c r="D6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="8">
         <v>45182.902777777781</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
+      <c r="F6" s="8">
+        <v>45182.986111111109</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9"/>
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="9"/>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6">
+        <v>45184</v>
+      </c>
+      <c r="F9" s="6">
+        <v>45184</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9"/>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="6">
+        <v>45184</v>
+      </c>
+      <c r="F10" s="6">
+        <v>45184</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="9"/>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="8">
+        <v>45185</v>
+      </c>
+      <c r="F11" s="8">
+        <v>45185</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="9"/>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="9"/>
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="6">
+        <v>45185</v>
+      </c>
+      <c r="F13" s="6">
+        <v>45185</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="9"/>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="6">
+        <v>45185</v>
+      </c>
+      <c r="F14" s="6">
+        <v>45185</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="9"/>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="6">
+        <v>45186</v>
+      </c>
+      <c r="F15" s="6">
+        <v>45186</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="6">
+        <v>45186</v>
+      </c>
+      <c r="F16" s="6">
+        <v>45186</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="9"/>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="8">
+        <v>45186</v>
+      </c>
+      <c r="F17" s="8">
+        <v>45186</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="9"/>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="9"/>
+      <c r="C19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="6">
+        <v>45186</v>
+      </c>
+      <c r="F19" s="6">
+        <v>45186</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="G6:G8"/>
+  <mergeCells count="17">
+    <mergeCell ref="B3:B19"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="G3:G5"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="D3:D8"/>
     <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="D6:D8"/>
     <mergeCell ref="E6:E8"/>
     <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add: documentacion de la retrospectiva
</commit_message>
<xml_diff>
--- a/Entrega 1/Documentacion/Registro de Horas.xlsx
+++ b/Entrega 1/Documentacion/Registro de Horas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fiore/Documents/Ingeniería de Software Ágil 2/Obligatorio/obligatorio-mazziotti-macedo-torres/Entrega 1/Documentacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Documents\Nico\Things\ORT\AAA\Ingeniería de software ágil 2\Obligatorio\obligatorio-mazziotti-macedo-torres\Entrega 1\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C471F7-76A8-9A49-8B70-97ECC75DDED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D225B8F-E1AE-4A15-961B-33A4727A4435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28120" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
   <si>
     <t>Integrante</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Análisis de Código</t>
+  </si>
+  <si>
+    <t>Retrospectiva</t>
   </si>
 </sst>
 </file>
@@ -122,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -145,25 +148,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -175,7 +181,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="46" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -492,316 +507,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G21"/>
+  <dimension ref="B1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="16.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.6640625" style="3"/>
-    <col min="7" max="7" width="16.6640625" style="2"/>
+    <col min="4" max="4" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.69921875" style="2"/>
+    <col min="7" max="7" width="16.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="4">
+    <row r="3" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="9">
         <v>45181.895138888889</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="9">
         <v>45182.020138888889</v>
       </c>
       <c r="G3" s="7">
         <v>0.125</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="8"/>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="8"/>
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
+    <row r="6" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="8"/>
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="9">
         <v>45182.902777777781</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="9">
         <v>45182.986111111109</v>
       </c>
       <c r="G6" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
+    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="8"/>
+      <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="8"/>
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8"/>
+      <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <v>45184</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="4">
         <v>45184</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
+    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="8"/>
+      <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <v>45184</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="4">
         <v>45184</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="8"/>
+      <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="9">
         <v>45185</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="9">
         <v>45185</v>
       </c>
       <c r="G11" s="7">
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="8"/>
+      <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="8"/>
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="4">
         <v>45185</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="4">
         <v>45185</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="5">
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="8"/>
+      <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="4">
         <v>45185</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="4">
         <v>45185</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="4"/>
-      <c r="C15" s="5" t="s">
+    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="4">
         <v>45186</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="4">
         <v>45186</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="5">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="5" t="s">
+    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8"/>
+      <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="4">
         <v>45186</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="4">
         <v>45186</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8"/>
+      <c r="C17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="9">
         <v>45186</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="9">
         <v>45186</v>
       </c>
       <c r="G17" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="4"/>
-      <c r="C18" s="5" t="s">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
+      <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5" t="s">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="8"/>
+      <c r="C19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="4">
         <v>45186</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="4">
         <v>45186</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="5">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G20" s="11">
-        <v>1.0416666666666667</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G21" s="1"/>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="8"/>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="9">
+        <v>45187</v>
+      </c>
+      <c r="F20" s="9">
+        <v>45187</v>
+      </c>
+      <c r="G20" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="8"/>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="8"/>
+      <c r="C22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="10">
+        <v>1.0625</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="21">
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="B3:B19"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="F17:F18"/>
@@ -816,7 +871,6 @@
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>